<commit_message>
last version of write to excel
</commit_message>
<xml_diff>
--- a/Data/Book1.xlsx
+++ b/Data/Book1.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Leo\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Leo\Projects\Accelify\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="15360" windowHeight="7365"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="15360" windowHeight="7365"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PSSP" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -396,12 +396,12 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>